<commit_message>
Run Black linter manually and all new dissertation copy
</commit_message>
<xml_diff>
--- a/literature.xlsx
+++ b/literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Downloads/msc-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD2DDA6-390C-6D42-B1A1-6C04510BB50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA146BB-16E1-7147-B3A1-60F3122644A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{A97D0385-DDF7-1B4E-86CF-EE7A373065A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="346">
   <si>
     <t>Neural networks for option pricing and hedging:
 a literature review</t>
@@ -1078,6 +1078,15 @@
   </si>
   <si>
     <t>Basket</t>
+  </si>
+  <si>
+    <t>Deep xVA solver -- A neural network based counterparty credit risk management framework</t>
+  </si>
+  <si>
+    <t>Alessandro Gnoatto, Athena Picarelli, Christoph Reisinger</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2005.02633</t>
   </si>
 </sst>
 </file>
@@ -1466,11 +1475,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF693112-DF4A-CA41-B82F-5732F185C14B}">
-  <dimension ref="A1:S104"/>
+  <dimension ref="A1:S105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H98" sqref="H98"/>
+      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3104,6 +3113,20 @@
       </c>
       <c r="L104">
         <v>150000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>343</v>
+      </c>
+      <c r="B105" t="s">
+        <v>344</v>
+      </c>
+      <c r="C105">
+        <v>2020</v>
+      </c>
+      <c r="D105" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>